<commit_message>
Complete la tarea #41: Tutorial ruby básico
</commit_message>
<xml_diff>
--- a/tspi/ciclo-2/logt2/20106065.xlsx
+++ b/tspi/ciclo-2/logt2/20106065.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>Name</t>
   </si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t>Comment</t>
+  </si>
+  <si>
+    <t>Cursar el tutorial básico de ruby.</t>
   </si>
 </sst>
 </file>
@@ -177,7 +180,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="165" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="166" xfId="0"/>
@@ -220,6 +223,9 @@
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
       <alignment horizontal="right" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
+      <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -241,18 +247,18 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="F2" activeCellId="0" pane="topLeft" sqref="F2"/>
+      <selection activeCell="H7" activeCellId="0" pane="topLeft" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.7333333333333"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="2" width="12.7333333333333"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="17.7176470588235"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="11.6588235294118"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="4" width="18.1333333333333"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="12.7333333333333"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="6" width="50.1137254901961"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="5" width="12.7333333333333"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.7960784313726"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="2" width="12.7960784313726"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="17.8078431372549"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="11.7137254901961"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="4" width="18.2235294117647"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="12.7960784313726"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="6" width="50.3607843137255"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="5" width="12.7960784313726"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.75" outlineLevel="0" r="1">
@@ -304,7 +310,7 @@
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.75" outlineLevel="0" r="5">
       <c r="E5" s="3" t="n">
         <f aca="false">SUM(E7:E14)/60</f>
-        <v>0</v>
+        <v>0.6</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="6">
@@ -333,12 +339,29 @@
         <v>14</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.75" outlineLevel="0" r="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="7">
+      <c r="A7" s="1" t="n">
+        <v>41933</v>
+      </c>
+      <c r="B7" s="2" t="n">
+        <v>0.576388888888889</v>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>0.601388888888889</v>
+      </c>
+      <c r="D7" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="E7" s="3" t="n">
         <f aca="false">((HOUR(C7)-HOUR(B7))*60)+(MINUTE(C7)-MINUTE(B7))-D7</f>
-        <v>0</v>
-      </c>
-      <c r="F7" s="18"/>
+        <v>36</v>
+      </c>
+      <c r="F7" s="18" t="n">
+        <v>41</v>
+      </c>
+      <c r="H7" s="19" t="s">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>